<commit_message>
pdf , brd and sch itt@26
</commit_message>
<xml_diff>
--- a/BMS_doc/AFE_BOARD_BOM.xlsx
+++ b/BMS_doc/AFE_BOARD_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GF_BMS\BMS_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6949E897-8189-4683-88B1-F9611BB46F5F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710129F7-A6B4-4125-B345-1FEE9BFE54B4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="4980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1559,7 +1559,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1602,27 +1602,18 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2011,8 +2002,8 @@
   <dimension ref="A1:L75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I46" sqref="I46"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,8 +2012,8 @@
     <col min="2" max="2" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="9" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="78.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="40.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="82.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.5703125" style="8" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" style="8" customWidth="1"/>
@@ -2119,7 +2110,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="7"/>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="17" t="s">
         <v>269</v>
       </c>
       <c r="E5" s="12" t="s">
@@ -2481,7 +2472,7 @@
       <c r="E15" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="16" t="s">
         <v>268</v>
       </c>
       <c r="G15" s="8"/>
@@ -2515,12 +2506,12 @@
       <c r="E16" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="8" t="s">
         <v>239</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="25" t="s">
+      <c r="I16" s="8" t="s">
         <v>240</v>
       </c>
       <c r="J16" s="1" t="s">
@@ -2655,7 +2646,7 @@
       <c r="E20" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="16" t="s">
         <v>276</v>
       </c>
       <c r="G20" s="8"/>
@@ -2793,7 +2784,7 @@
       <c r="E24" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="16" t="s">
         <v>299</v>
       </c>
       <c r="J24" s="1" t="s">
@@ -2816,14 +2807,10 @@
       <c r="D25" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="F25" s="18"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="16"/>
+      <c r="F25" s="16"/>
       <c r="K25" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2843,20 +2830,19 @@
       <c r="D26" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="F26" s="25" t="s">
+      <c r="F26" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25" t="s">
+      <c r="H26" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="I26" s="25" t="s">
+      <c r="I26" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="J26" s="25" t="s">
+      <c r="J26" s="8" t="s">
         <v>244</v>
       </c>
       <c r="K26" s="1">
@@ -2980,16 +2966,16 @@
       <c r="D30" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="F30" s="25" t="s">
+      <c r="F30" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="H30" s="25" t="s">
+      <c r="H30" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I30" s="25" t="s">
+      <c r="I30" s="8" t="s">
         <v>245</v>
       </c>
       <c r="J30" s="1" t="s">
@@ -3048,17 +3034,16 @@
       <c r="D32" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="F32" s="25" t="s">
+      <c r="F32" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25" t="s">
+      <c r="H32" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I32" s="25" t="s">
+      <c r="I32" s="8" t="s">
         <v>245</v>
       </c>
       <c r="J32" s="1" t="s">
@@ -3083,17 +3068,16 @@
       <c r="D33" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E33" s="25" t="s">
+      <c r="E33" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F33" s="25" t="s">
+      <c r="F33" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25" t="s">
+      <c r="H33" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I33" s="25" t="s">
+      <c r="I33" s="8" t="s">
         <v>66</v>
       </c>
       <c r="J33" s="1" t="s">
@@ -3124,7 +3108,7 @@
       <c r="F34" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="I34" s="25" t="s">
+      <c r="I34" s="8" t="s">
         <v>210</v>
       </c>
       <c r="J34" s="1" t="s">
@@ -3335,7 +3319,7 @@
       <c r="F41" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="I41" s="21"/>
+      <c r="I41" s="19"/>
       <c r="J41" s="1" t="s">
         <v>80</v>
       </c>
@@ -3473,7 +3457,7 @@
       <c r="F46" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="I46" s="23" t="s">
+      <c r="I46" s="20" t="s">
         <v>310</v>
       </c>
       <c r="J46" s="1" t="s">
@@ -3601,7 +3585,7 @@
         <v>175</v>
       </c>
       <c r="F50" s="6"/>
-      <c r="I50" s="22" t="s">
+      <c r="I50" s="18" t="s">
         <v>249</v>
       </c>
       <c r="J50" s="1" t="s">
@@ -4061,7 +4045,7 @@
         <v>9</v>
       </c>
       <c r="C64" s="7"/>
-      <c r="D64" s="19" t="s">
+      <c r="D64" s="17" t="s">
         <v>314</v>
       </c>
       <c r="E64" s="12" t="s">
@@ -4164,7 +4148,7 @@
       <c r="B67" s="2">
         <v>1</v>
       </c>
-      <c r="D67" s="16" t="s">
+      <c r="D67" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E67" s="1" t="s">
@@ -4233,13 +4217,13 @@
       <c r="E69" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="F69" s="20" t="s">
+      <c r="F69" s="21" t="s">
         <v>291</v>
       </c>
       <c r="H69" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="I69" s="20" t="s">
+      <c r="I69" s="21" t="s">
         <v>290</v>
       </c>
       <c r="J69" s="1" t="s">
@@ -4267,7 +4251,7 @@
       <c r="E70" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F70" s="17" t="s">
+      <c r="F70" s="16" t="s">
         <v>289</v>
       </c>
       <c r="I70" s="8" t="s">
@@ -4335,7 +4319,7 @@
       <c r="F72" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="H72" s="25" t="s">
+      <c r="H72" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I72" s="8" t="s">
@@ -4369,7 +4353,7 @@
       <c r="F73" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="H73" s="25" t="s">
+      <c r="H73" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I73" s="8" t="s">
@@ -4697,14 +4681,14 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{817A1FC8-D3A3-4B4B-9419-3DB2734E9FAB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="c4672b8b-43e2-4139-8cd1-27ad03f081e7"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="f8cd1e16-0731-4200-9ee6-df6e2184771e"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="1f7e2bd1-5fdf-4d6b-8b99-ef650a991a33"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>

</xml_diff>